<commit_message>
added energy plots for linear model
</commit_message>
<xml_diff>
--- a/matlab/2_output/Simulation_Results.xlsx
+++ b/matlab/2_output/Simulation_Results.xlsx
@@ -10,6 +10,7 @@
     <sheet name="WeOhSweep20241109T154213.mat" sheetId="3" r:id="rId5"/>
     <sheet name="WeOhSweep20241109T153735.mat" sheetId="4" r:id="rId6"/>
     <sheet name="WeOhSweep20241109T155008.mat" sheetId="5" r:id="rId7"/>
+    <sheet name="energyPlot20250703T094134.mat" sheetId="6" r:id="rId8"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="125725" fullCalcOnLoad="true"/>
@@ -17,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="7">
   <si>
     <t>Time_ms</t>
   </si>
@@ -58,7 +59,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="17">
+  <borders count="21">
     <border>
       <left/>
       <right/>
@@ -82,11 +83,15 @@
     <border/>
     <border/>
     <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="true"/>
@@ -104,6 +109,10 @@
     <xf numFmtId="22" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -7657,4 +7666,1779 @@
     </row>
   </sheetData>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:E217"/>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="15.7109375" customWidth="true"/>
+    <col min="2" max="2" width="16" customWidth="true"/>
+    <col min="4" max="4" width="10.85546875" customWidth="true"/>
+    <col min="5" max="5" width="13.7109375" customWidth="true"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="17" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="19" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="19" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="D2" s="19" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2">
+        <v>0.2540957506835434</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3">
+        <v>0.00085568390845986407</v>
+      </c>
+      <c r="B3">
+        <v>7.5352284766898116e-06</v>
+      </c>
+      <c r="D3" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="E3">
+        <v>0.030376704936702505</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4">
+        <v>0.0017113678169197316</v>
+      </c>
+      <c r="B4">
+        <v>1.0654721957941682e-05</v>
+      </c>
+      <c r="D4" s="19" t="s">
+        <v>5</v>
+      </c>
+      <c r="E4">
+        <v>0.0189</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5">
+        <v>0.0025670517253795992</v>
+      </c>
+      <c r="B5">
+        <v>1.3047233016840939e-05</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6">
+        <v>0.0034227356338394632</v>
+      </c>
+      <c r="B6">
+        <v>1.5063241031070128e-05</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7">
+        <v>0.0042784195422993273</v>
+      </c>
+      <c r="B7">
+        <v>1.6838524783184499e-05</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8">
+        <v>0.0051341034507591948</v>
+      </c>
+      <c r="B8">
+        <v>1.8442731438606749e-05</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9">
+        <v>0.0059897873592190624</v>
+      </c>
+      <c r="B9">
+        <v>1.9917241336773536e-05</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10">
+        <v>0.0068454712676789264</v>
+      </c>
+      <c r="B10">
+        <v>2.128902039796151e-05</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11">
+        <v>0.0077011551761387905</v>
+      </c>
+      <c r="B11">
+        <v>2.257680220951963e-05</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12">
+        <v>0.0085568390845986581</v>
+      </c>
+      <c r="B12">
+        <v>2.3794228753088662e-05</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13">
+        <v>0.0094125229930585256</v>
+      </c>
+      <c r="B13">
+        <v>2.4951600255742767e-05</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14">
+        <v>0.01026820690151839</v>
+      </c>
+      <c r="B14">
+        <v>2.6056920234163877e-05</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15">
+        <v>0.011123890809978255</v>
+      </c>
+      <c r="B15">
+        <v>2.7116554468316671e-05</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16">
+        <v>0.011979574718438121</v>
+      </c>
+      <c r="B16">
+        <v>2.8135665119740738e-05</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17">
+        <v>0.012835258626897985</v>
+      </c>
+      <c r="B17">
+        <v>2.9118507217185578e-05</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18">
+        <v>0.013690942535357851</v>
+      </c>
+      <c r="B18">
+        <v>3.0068637360060607e-05</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19">
+        <v>0.014546626443817717</v>
+      </c>
+      <c r="B19">
+        <v>3.0989064460013761e-05</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20">
+        <v>0.015402310352277584</v>
+      </c>
+      <c r="B20">
+        <v>3.1882361060329235e-05</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21">
+        <v>0.01625799426073745</v>
+      </c>
+      <c r="B21">
+        <v>3.2750747147038076e-05</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22">
+        <v>0.017113678169197316</v>
+      </c>
+      <c r="B22">
+        <v>3.3596154330608719e-05</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23">
+        <v>0.017969362077657182</v>
+      </c>
+      <c r="B23">
+        <v>3.4420275741292279e-05</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24">
+        <v>0.018825045986117048</v>
+      </c>
+      <c r="B24">
+        <v>3.5224605342931841e-05</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25">
+        <v>0.019680729894576917</v>
+      </c>
+      <c r="B25">
+        <v>3.601046928542316e-05</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26">
+        <v>0.020536413803036779</v>
+      </c>
+      <c r="B26">
+        <v>3.6779051182076231e-05</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27">
+        <v>0.021392097711496645</v>
+      </c>
+      <c r="B27">
+        <v>3.7531412691651588e-05</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28">
+        <v>0.022247781619956511</v>
+      </c>
+      <c r="B28">
+        <v>3.8268510429091701e-05</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29">
+        <v>0.02310346552841638</v>
+      </c>
+      <c r="B29">
+        <v>3.8991209975045387e-05</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30">
+        <v>0.023959149436876243</v>
+      </c>
+      <c r="B30">
+        <v>3.9700297570339283e-05</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31">
+        <v>0.024814833345336108</v>
+      </c>
+      <c r="B31">
+        <v>4.0396489946529335e-05</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32">
+        <v>0.024814833345336108</v>
+      </c>
+      <c r="B32">
+        <v>4.0385019521540485e-05</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33">
+        <v>0.034836051146696731</v>
+      </c>
+      <c r="B33">
+        <v>4.804864699136778e-05</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34">
+        <v>0.045143589456667653</v>
+      </c>
+      <c r="B34">
+        <v>5.6015704065283713e-05</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35">
+        <v>0.054878486749417962</v>
+      </c>
+      <c r="B35">
+        <v>6.2736521478583938e-05</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36">
+        <v>0.065186025059388905</v>
+      </c>
+      <c r="B36">
+        <v>6.880354634109339e-05</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37">
+        <v>0.074920922352139208</v>
+      </c>
+      <c r="B37">
+        <v>7.3782853504973314e-05</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38">
+        <v>0.085228460662110136</v>
+      </c>
+      <c r="B38">
+        <v>7.848761378357931e-05</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39">
+        <v>0.094963357954860453</v>
+      </c>
+      <c r="B39">
+        <v>8.2388766734650554e-05</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40">
+        <v>0.10527089626483137</v>
+      </c>
+      <c r="B40">
+        <v>8.6221199736824885e-05</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41">
+        <v>0.11500579355758168</v>
+      </c>
+      <c r="B41">
+        <v>8.9512489917451977e-05</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42">
+        <v>0.12531333186755259</v>
+      </c>
+      <c r="B42">
+        <v>9.2816285494549917e-05</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43">
+        <v>0.1350482291603029</v>
+      </c>
+      <c r="B43">
+        <v>9.559781611719074e-05</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44">
+        <v>0.14535576747027384</v>
+      </c>
+      <c r="B44">
+        <v>9.8523859365430479e-05</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45">
+        <v>0.15509066476302416</v>
+      </c>
+      <c r="B45">
+        <v>0.00010097555694542895</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46">
+        <v>0.16482556205577445</v>
+      </c>
+      <c r="B46">
+        <v>0.00010341699864353417</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47">
+        <v>0.17513310036574539</v>
+      </c>
+      <c r="B47">
+        <v>0.00010580720978928753</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48">
+        <v>0.18486799765849582</v>
+      </c>
+      <c r="B48">
+        <v>0.00010789647880267201</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49">
+        <v>0.19517553596846704</v>
+      </c>
+      <c r="B49">
+        <v>0.00011017122899110593</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50">
+        <v>0.20491043326121766</v>
+      </c>
+      <c r="B50">
+        <v>0.00011203805203964327</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51">
+        <v>0.21521797157118888</v>
+      </c>
+      <c r="B51">
+        <v>0.00011396415580370499</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52">
+        <v>0.2249528688639395</v>
+      </c>
+      <c r="B52">
+        <v>0.00011579148636579522</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53">
+        <v>0.23526040717391075</v>
+      </c>
+      <c r="B53">
+        <v>0.00011756534479671198</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54">
+        <v>0.24499530446666132</v>
+      </c>
+      <c r="B54">
+        <v>0.00011909474673371097</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55">
+        <v>0.25530284277663257</v>
+      </c>
+      <c r="B55">
+        <v>0.0001208203845849906</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56">
+        <v>0.26503774006938319</v>
+      </c>
+      <c r="B56">
+        <v>0.0001222248194378948</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57">
+        <v>0.27534527837935441</v>
+      </c>
+      <c r="B57">
+        <v>0.00012362894618584493</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58">
+        <v>0.28508017567210503</v>
+      </c>
+      <c r="B58">
+        <v>0.00012493209158701484</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59">
+        <v>0.29481507296485565</v>
+      </c>
+      <c r="B59">
+        <v>0.00012624396465188572</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60">
+        <v>0.30512261127482687</v>
+      </c>
+      <c r="B60">
+        <v>0.00012747255210918853</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61">
+        <v>0.31485750856757749</v>
+      </c>
+      <c r="B61">
+        <v>0.00012854768852599288</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62">
+        <v>0.32516504687754877</v>
+      </c>
+      <c r="B62">
+        <v>0.00012965164676893758</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63">
+        <v>0.33489994417029934</v>
+      </c>
+      <c r="B63">
+        <v>0.00013073781348374282</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64">
+        <v>0.34520748248027011</v>
+      </c>
+      <c r="B64">
+        <v>0.00013170397505042657</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65">
+        <v>0.35494237977302018</v>
+      </c>
+      <c r="B65">
+        <v>0.00013254789967767741</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66">
+        <v>0.36524991808299079</v>
+      </c>
+      <c r="B66">
+        <v>0.00013336433237065871</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67">
+        <v>0.3749848153757408</v>
+      </c>
+      <c r="B67">
+        <v>0.00013413186453148634</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68">
+        <v>0.38529235368571146</v>
+      </c>
+      <c r="B68">
+        <v>0.00013497786772795919</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69">
+        <v>0.39502725097846142</v>
+      </c>
+      <c r="B69">
+        <v>0.00013568889591836596</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70">
+        <v>0.40533478928843208</v>
+      </c>
+      <c r="B70">
+        <v>0.00013632720001062411</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71">
+        <v>0.41506968658118204</v>
+      </c>
+      <c r="B71">
+        <v>0.00013684297776520311</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72">
+        <v>0.42537722489115271</v>
+      </c>
+      <c r="B72">
+        <v>0.00013739365793196971</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73">
+        <v>0.43511212218390266</v>
+      </c>
+      <c r="B73">
+        <v>0.00013785230934914371</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74">
+        <v>0.44484701947665273</v>
+      </c>
+      <c r="B74">
+        <v>0.00013828208746549314</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75">
+        <v>0.45515455778662328</v>
+      </c>
+      <c r="B75">
+        <v>0.00013875321167206641</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76">
+        <v>0.46488945507937335</v>
+      </c>
+      <c r="B76">
+        <v>0.00013916865917935417</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77">
+        <v>0.4751969933893439</v>
+      </c>
+      <c r="B77">
+        <v>0.0001394746112488569</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78">
+        <v>0.48493189068209397</v>
+      </c>
+      <c r="B78">
+        <v>0.00013973237197590082</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79">
+        <v>0.49523942899206458</v>
+      </c>
+      <c r="B79">
+        <v>0.00013993341487591787</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80">
+        <v>0.50497432628481453</v>
+      </c>
+      <c r="B80">
+        <v>0.00014013149049557858</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81">
+        <v>0.51528186459478509</v>
+      </c>
+      <c r="B81">
+        <v>0.00014027654554815634</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82">
+        <v>0.52501676188753521</v>
+      </c>
+      <c r="B82">
+        <v>0.00014037086812049223</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83">
+        <v>0.53532430019750576</v>
+      </c>
+      <c r="B83">
+        <v>0.0001404844171565668</v>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84">
+        <v>0.54505919749025578</v>
+      </c>
+      <c r="B84">
+        <v>0.00014054788847055245</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85">
+        <v>0.55536673580022633</v>
+      </c>
+      <c r="B85">
+        <v>0.00014060514361156478</v>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86">
+        <v>0.56510163309297645</v>
+      </c>
+      <c r="B86">
+        <v>0.00014061089319640136</v>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87">
+        <v>0.57483653038572646</v>
+      </c>
+      <c r="B87">
+        <v>0.00014058753245977407</v>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88">
+        <v>0.58514406869569702</v>
+      </c>
+      <c r="B88">
+        <v>0.00014056097108927428</v>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89">
+        <v>0.59487896598844703</v>
+      </c>
+      <c r="B89">
+        <v>0.0001404805513459178</v>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90">
+        <v>0.60518650429841769</v>
+      </c>
+      <c r="B90">
+        <v>0.00014039891870222919</v>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91">
+        <v>0.6149214015911677</v>
+      </c>
+      <c r="B91">
+        <v>0.00014030569272652067</v>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92">
+        <v>0.62522893990113826</v>
+      </c>
+      <c r="B92">
+        <v>0.00014016935433790352</v>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93">
+        <v>0.63496383719388827</v>
+      </c>
+      <c r="B93">
+        <v>0.00014001977138662096</v>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94">
+        <v>0.64527137550385893</v>
+      </c>
+      <c r="B94">
+        <v>0.00013982914387237265</v>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95">
+        <v>0.65500627279660961</v>
+      </c>
+      <c r="B95">
+        <v>0.00013962363127864577</v>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96">
+        <v>0.66531381110658128</v>
+      </c>
+      <c r="B96">
+        <v>0.00013937918540783128</v>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97">
+        <v>0.67504870839933262</v>
+      </c>
+      <c r="B97">
+        <v>0.00013916187872044185</v>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98">
+        <v>0.68535624670930451</v>
+      </c>
+      <c r="B98">
+        <v>0.00013886418731014831</v>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99">
+        <v>0.69509114400205563</v>
+      </c>
+      <c r="B99">
+        <v>0.00013859205789753208</v>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100">
+        <v>0.70482604129480675</v>
+      </c>
+      <c r="B100">
+        <v>0.00013829241931076112</v>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101">
+        <v>0.71513357960477864</v>
+      </c>
+      <c r="B101">
+        <v>0.00013795963283729087</v>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102">
+        <v>0.72486847689752998</v>
+      </c>
+      <c r="B102">
+        <v>0.00013760693399367978</v>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103">
+        <v>0.73517601520750187</v>
+      </c>
+      <c r="B103">
+        <v>0.00013726702065614696</v>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104">
+        <v>0.74491091250025299</v>
+      </c>
+      <c r="B104">
+        <v>0.00013690580503763504</v>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105">
+        <v>0.75521845081022487</v>
+      </c>
+      <c r="B105">
+        <v>0.0001365166292286652</v>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106">
+        <v>0.76495334810297599</v>
+      </c>
+      <c r="B106">
+        <v>0.0001361475726558655</v>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107">
+        <v>0.77526088641294788</v>
+      </c>
+      <c r="B107">
+        <v>0.00013575258294701921</v>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108">
+        <v>0.784995783705699</v>
+      </c>
+      <c r="B108">
+        <v>0.0001353753154985079</v>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109">
+        <v>0.79530332201567089</v>
+      </c>
+      <c r="B109">
+        <v>0.00013493077625362617</v>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110">
+        <v>0.80503821930842223</v>
+      </c>
+      <c r="B110">
+        <v>0.00013453892645750283</v>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111">
+        <v>0.8153457576183939</v>
+      </c>
+      <c r="B111">
+        <v>0.00013410750879333698</v>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112">
+        <v>0.82508065491114524</v>
+      </c>
+      <c r="B112">
+        <v>0.00013364766662683788</v>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113">
+        <v>0.83481555220389636</v>
+      </c>
+      <c r="B113">
+        <v>0.0001332026913795805</v>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114">
+        <v>0.84512309051386825</v>
+      </c>
+      <c r="B114">
+        <v>0.00013274019120014202</v>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115">
+        <v>0.85485798780661937</v>
+      </c>
+      <c r="B115">
+        <v>0.00013233359529630153</v>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116">
+        <v>0.86516552611659125</v>
+      </c>
+      <c r="B116">
+        <v>0.00013182209531541799</v>
+      </c>
+    </row>
+    <row r="117">
+      <c r="A117">
+        <v>0.8749004234093426</v>
+      </c>
+      <c r="B117">
+        <v>0.00013130991385229039</v>
+      </c>
+    </row>
+    <row r="118">
+      <c r="A118">
+        <v>0.88520796171931448</v>
+      </c>
+      <c r="B118">
+        <v>0.00013073542144080282</v>
+      </c>
+    </row>
+    <row r="119">
+      <c r="A119">
+        <v>0.89494285901206561</v>
+      </c>
+      <c r="B119">
+        <v>0.00013016519087893902</v>
+      </c>
+    </row>
+    <row r="120">
+      <c r="A120">
+        <v>0.90525039732203749</v>
+      </c>
+      <c r="B120">
+        <v>0.00012957917078844556</v>
+      </c>
+    </row>
+    <row r="121">
+      <c r="A121">
+        <v>0.91498529461478861</v>
+      </c>
+      <c r="B121">
+        <v>0.00012899996092166402</v>
+      </c>
+    </row>
+    <row r="122">
+      <c r="A122">
+        <v>0.9252928329247605</v>
+      </c>
+      <c r="B122">
+        <v>0.00012844244756355814</v>
+      </c>
+    </row>
+    <row r="123">
+      <c r="A123">
+        <v>0.93502773021751162</v>
+      </c>
+      <c r="B123">
+        <v>0.00012789752677749784</v>
+      </c>
+    </row>
+    <row r="124">
+      <c r="A124">
+        <v>0.94533526852748351</v>
+      </c>
+      <c r="B124">
+        <v>0.00012743373008858685</v>
+      </c>
+    </row>
+    <row r="125">
+      <c r="A125">
+        <v>0.95507016582023485</v>
+      </c>
+      <c r="B125">
+        <v>0.00012700986474016758</v>
+      </c>
+    </row>
+    <row r="126">
+      <c r="A126">
+        <v>0.96537770413020652</v>
+      </c>
+      <c r="B126">
+        <v>0.00012653725893924084</v>
+      </c>
+    </row>
+    <row r="127">
+      <c r="A127">
+        <v>0.97511260142295786</v>
+      </c>
+      <c r="B127">
+        <v>0.00012613936526478548</v>
+      </c>
+    </row>
+    <row r="128">
+      <c r="A128">
+        <v>0.98484749871570898</v>
+      </c>
+      <c r="B128">
+        <v>0.0001257212783813065</v>
+      </c>
+    </row>
+    <row r="129">
+      <c r="A129">
+        <v>0.99515503702568087</v>
+      </c>
+      <c r="B129">
+        <v>0.0001253415828195516</v>
+      </c>
+    </row>
+    <row r="130">
+      <c r="A130">
+        <v>1.0048899343184321</v>
+      </c>
+      <c r="B130">
+        <v>0.00012503897266681301</v>
+      </c>
+    </row>
+    <row r="131">
+      <c r="A131">
+        <v>1.0151974726284039</v>
+      </c>
+      <c r="B131">
+        <v>0.00012477789143768589</v>
+      </c>
+    </row>
+    <row r="132">
+      <c r="A132">
+        <v>1.024932369921155</v>
+      </c>
+      <c r="B132">
+        <v>0.00012460184055960348</v>
+      </c>
+    </row>
+    <row r="133">
+      <c r="A133">
+        <v>1.035239908231127</v>
+      </c>
+      <c r="B133">
+        <v>0.00012441177541673475</v>
+      </c>
+    </row>
+    <row r="134">
+      <c r="A134">
+        <v>1.0449748055238783</v>
+      </c>
+      <c r="B134">
+        <v>0.00012432522020240644</v>
+      </c>
+    </row>
+    <row r="135">
+      <c r="A135">
+        <v>1.0552823438338501</v>
+      </c>
+      <c r="B135">
+        <v>0.00012424811008656105</v>
+      </c>
+    </row>
+    <row r="136">
+      <c r="A136">
+        <v>1.0650172411266012</v>
+      </c>
+      <c r="B136">
+        <v>0.00012419253101034184</v>
+      </c>
+    </row>
+    <row r="137">
+      <c r="A137">
+        <v>1.0753247794365732</v>
+      </c>
+      <c r="B137">
+        <v>0.0001241366160380023</v>
+      </c>
+    </row>
+    <row r="138">
+      <c r="A138">
+        <v>1.0850596767293244</v>
+      </c>
+      <c r="B138">
+        <v>0.00012409847357636628</v>
+      </c>
+    </row>
+    <row r="139">
+      <c r="A139">
+        <v>1.0953672150392961</v>
+      </c>
+      <c r="B139">
+        <v>0.00012398841758398061</v>
+      </c>
+    </row>
+    <row r="140">
+      <c r="A140">
+        <v>1.1051021123320472</v>
+      </c>
+      <c r="B140">
+        <v>0.00012392913102527407</v>
+      </c>
+    </row>
+    <row r="141">
+      <c r="A141">
+        <v>1.1148370096247986</v>
+      </c>
+      <c r="B141">
+        <v>0.00012380309740607615</v>
+      </c>
+    </row>
+    <row r="142">
+      <c r="A142">
+        <v>1.1251445479347706</v>
+      </c>
+      <c r="B142">
+        <v>0.00012363756197275577</v>
+      </c>
+    </row>
+    <row r="143">
+      <c r="A143">
+        <v>1.1348794452275217</v>
+      </c>
+      <c r="B143">
+        <v>0.00012348135083329489</v>
+      </c>
+    </row>
+    <row r="144">
+      <c r="A144">
+        <v>1.1451869835374935</v>
+      </c>
+      <c r="B144">
+        <v>0.00012321956428452914</v>
+      </c>
+    </row>
+    <row r="145">
+      <c r="A145">
+        <v>1.1549218808302446</v>
+      </c>
+      <c r="B145">
+        <v>0.0001229579588811751</v>
+      </c>
+    </row>
+    <row r="146">
+      <c r="A146">
+        <v>1.1652294191402166</v>
+      </c>
+      <c r="B146">
+        <v>0.00012258719001162198</v>
+      </c>
+    </row>
+    <row r="147">
+      <c r="A147">
+        <v>1.1749643164329677</v>
+      </c>
+      <c r="B147">
+        <v>0.00012222069016990227</v>
+      </c>
+    </row>
+    <row r="148">
+      <c r="A148">
+        <v>1.1852718547429395</v>
+      </c>
+      <c r="B148">
+        <v>0.00012178408313281205</v>
+      </c>
+    </row>
+    <row r="149">
+      <c r="A149">
+        <v>1.1950067520356908</v>
+      </c>
+      <c r="B149">
+        <v>0.00012135756640081946</v>
+      </c>
+    </row>
+    <row r="150">
+      <c r="A150">
+        <v>1.2053142903456628</v>
+      </c>
+      <c r="B150">
+        <v>0.00012077574941438068</v>
+      </c>
+    </row>
+    <row r="151">
+      <c r="A151">
+        <v>1.215049187638414</v>
+      </c>
+      <c r="B151">
+        <v>0.00012011812135783839</v>
+      </c>
+    </row>
+    <row r="152">
+      <c r="A152">
+        <v>1.2253567259483857</v>
+      </c>
+      <c r="B152">
+        <v>0.00011935841039591257</v>
+      </c>
+    </row>
+    <row r="153">
+      <c r="A153">
+        <v>1.2350916232411369</v>
+      </c>
+      <c r="B153">
+        <v>0.00011851574540017149</v>
+      </c>
+    </row>
+    <row r="154">
+      <c r="A154">
+        <v>1.244826520533888</v>
+      </c>
+      <c r="B154">
+        <v>0.00011767290818376126</v>
+      </c>
+    </row>
+    <row r="155">
+      <c r="A155">
+        <v>1.25513405884386</v>
+      </c>
+      <c r="B155">
+        <v>0.00011680736756145266</v>
+      </c>
+    </row>
+    <row r="156">
+      <c r="A156">
+        <v>1.2648689561366113</v>
+      </c>
+      <c r="B156">
+        <v>0.00011590556463076861</v>
+      </c>
+    </row>
+    <row r="157">
+      <c r="A157">
+        <v>1.2751764944465831</v>
+      </c>
+      <c r="B157">
+        <v>0.00011476375767869986</v>
+      </c>
+    </row>
+    <row r="158">
+      <c r="A158">
+        <v>1.284911391739334</v>
+      </c>
+      <c r="B158">
+        <v>0.0001135984150345175</v>
+      </c>
+    </row>
+    <row r="159">
+      <c r="A159">
+        <v>1.295218930049306</v>
+      </c>
+      <c r="B159">
+        <v>0.00011240026251429873</v>
+      </c>
+    </row>
+    <row r="160">
+      <c r="A160">
+        <v>1.3049538273420573</v>
+      </c>
+      <c r="B160">
+        <v>0.00011131576426008894</v>
+      </c>
+    </row>
+    <row r="161">
+      <c r="A161">
+        <v>1.3152613656520289</v>
+      </c>
+      <c r="B161">
+        <v>0.00011000288146612592</v>
+      </c>
+    </row>
+    <row r="162">
+      <c r="A162">
+        <v>1.3249962629447802</v>
+      </c>
+      <c r="B162">
+        <v>0.00010868050979075797</v>
+      </c>
+    </row>
+    <row r="163">
+      <c r="A163">
+        <v>1.3353038012547522</v>
+      </c>
+      <c r="B163">
+        <v>0.000107209050902532</v>
+      </c>
+    </row>
+    <row r="164">
+      <c r="A164">
+        <v>1.3450386985475034</v>
+      </c>
+      <c r="B164">
+        <v>0.00010590441045178383</v>
+      </c>
+    </row>
+    <row r="165">
+      <c r="A165">
+        <v>1.3553462368574751</v>
+      </c>
+      <c r="B165">
+        <v>0.0001044088295077991</v>
+      </c>
+    </row>
+    <row r="166">
+      <c r="A166">
+        <v>1.3650811341502262</v>
+      </c>
+      <c r="B166">
+        <v>0.0001028464984917604</v>
+      </c>
+    </row>
+    <row r="167">
+      <c r="A167">
+        <v>1.3748160314429776</v>
+      </c>
+      <c r="B167">
+        <v>0.00010129108222845194</v>
+      </c>
+    </row>
+    <row r="168">
+      <c r="A168">
+        <v>1.3851235697529494</v>
+      </c>
+      <c r="B168">
+        <v>9.9766027779073644e-05</v>
+      </c>
+    </row>
+    <row r="169">
+      <c r="A169">
+        <v>1.3948584670457007</v>
+      </c>
+      <c r="B169">
+        <v>9.8087608680097276e-05</v>
+      </c>
+    </row>
+    <row r="170">
+      <c r="A170">
+        <v>1.4051660053556725</v>
+      </c>
+      <c r="B170">
+        <v>9.6296589636399169e-05</v>
+      </c>
+    </row>
+    <row r="171">
+      <c r="A171">
+        <v>1.4149009026484236</v>
+      </c>
+      <c r="B171">
+        <v>9.4701581170912542e-05</v>
+      </c>
+    </row>
+    <row r="172">
+      <c r="A172">
+        <v>1.4252084409583956</v>
+      </c>
+      <c r="B172">
+        <v>9.2883599199954762e-05</v>
+      </c>
+    </row>
+    <row r="173">
+      <c r="A173">
+        <v>1.4349433382511467</v>
+      </c>
+      <c r="B173">
+        <v>9.1008591604136875e-05</v>
+      </c>
+    </row>
+    <row r="174">
+      <c r="A174">
+        <v>1.4452508765611185</v>
+      </c>
+      <c r="B174">
+        <v>8.9164270803440302e-05</v>
+      </c>
+    </row>
+    <row r="175">
+      <c r="A175">
+        <v>1.4549857738538698</v>
+      </c>
+      <c r="B175">
+        <v>8.7375664496298558e-05</v>
+      </c>
+    </row>
+    <row r="176">
+      <c r="A176">
+        <v>1.4652933121638416</v>
+      </c>
+      <c r="B176">
+        <v>8.5305925872935365e-05</v>
+      </c>
+    </row>
+    <row r="177">
+      <c r="A177">
+        <v>1.475028209456593</v>
+      </c>
+      <c r="B177">
+        <v>8.3441810484594764e-05</v>
+      </c>
+    </row>
+    <row r="178">
+      <c r="A178">
+        <v>1.4853357477665647</v>
+      </c>
+      <c r="B178">
+        <v>8.1417895350567934e-05</v>
+      </c>
+    </row>
+    <row r="179">
+      <c r="A179">
+        <v>1.4950706450593159</v>
+      </c>
+      <c r="B179">
+        <v>7.932688457315117e-05</v>
+      </c>
+    </row>
+    <row r="180">
+      <c r="A180">
+        <v>1.5053781833692879</v>
+      </c>
+      <c r="B180">
+        <v>7.7215778529117433e-05</v>
+      </c>
+    </row>
+    <row r="181">
+      <c r="A181">
+        <v>1.515113080662039</v>
+      </c>
+      <c r="B181">
+        <v>7.5186992715934299e-05</v>
+      </c>
+    </row>
+    <row r="182">
+      <c r="A182">
+        <v>1.5248479779547903</v>
+      </c>
+      <c r="B182">
+        <v>7.2967341221523728e-05</v>
+      </c>
+    </row>
+    <row r="183">
+      <c r="A183">
+        <v>1.5351555162647619</v>
+      </c>
+      <c r="B183">
+        <v>7.0763998472131865e-05</v>
+      </c>
+    </row>
+    <row r="184">
+      <c r="A184">
+        <v>1.5448904135575132</v>
+      </c>
+      <c r="B184">
+        <v>6.8556099994736028e-05</v>
+      </c>
+    </row>
+    <row r="185">
+      <c r="A185">
+        <v>1.5551979518674852</v>
+      </c>
+      <c r="B185">
+        <v>6.6102046103712074e-05</v>
+      </c>
+    </row>
+    <row r="186">
+      <c r="A186">
+        <v>1.5649328491602363</v>
+      </c>
+      <c r="B186">
+        <v>6.3901306659575104e-05</v>
+      </c>
+    </row>
+    <row r="187">
+      <c r="A187">
+        <v>1.5752403874702081</v>
+      </c>
+      <c r="B187">
+        <v>6.130400039140244e-05</v>
+      </c>
+    </row>
+    <row r="188">
+      <c r="A188">
+        <v>1.5849752847629592</v>
+      </c>
+      <c r="B188">
+        <v>5.8885749389845354e-05</v>
+      </c>
+    </row>
+    <row r="189">
+      <c r="A189">
+        <v>1.5952828230729312</v>
+      </c>
+      <c r="B189">
+        <v>5.6280545999164646e-05</v>
+      </c>
+    </row>
+    <row r="190">
+      <c r="A190">
+        <v>1.6050177203656826</v>
+      </c>
+      <c r="B190">
+        <v>5.3631122196263018e-05</v>
+      </c>
+    </row>
+    <row r="191">
+      <c r="A191">
+        <v>1.6153252586756541</v>
+      </c>
+      <c r="B191">
+        <v>5.0925926812498714e-05</v>
+      </c>
+    </row>
+    <row r="192">
+      <c r="A192">
+        <v>1.6250601559684055</v>
+      </c>
+      <c r="B192">
+        <v>4.8072937335638641e-05</v>
+      </c>
+    </row>
+    <row r="193">
+      <c r="A193">
+        <v>1.6353676942783775</v>
+      </c>
+      <c r="B193">
+        <v>4.5070215692948779e-05</v>
+      </c>
+    </row>
+    <row r="194">
+      <c r="A194">
+        <v>1.6451025915711286</v>
+      </c>
+      <c r="B194">
+        <v>4.1968972456078678e-05</v>
+      </c>
+    </row>
+    <row r="195">
+      <c r="A195">
+        <v>1.6548374888638797</v>
+      </c>
+      <c r="B195">
+        <v>3.8799102280238484e-05</v>
+      </c>
+    </row>
+    <row r="196">
+      <c r="A196">
+        <v>1.6651450271738515</v>
+      </c>
+      <c r="B196">
+        <v>3.5042499603982711e-05</v>
+      </c>
+    </row>
+    <row r="197">
+      <c r="A197">
+        <v>1.6748799244666028</v>
+      </c>
+      <c r="B197">
+        <v>3.1182180956965355e-05</v>
+      </c>
+    </row>
+    <row r="198">
+      <c r="A198">
+        <v>1.6851874627765748</v>
+      </c>
+      <c r="B198">
+        <v>2.5861481646837023e-05</v>
+      </c>
+    </row>
+    <row r="199">
+      <c r="A199">
+        <v>1.694922360069326</v>
+      </c>
+      <c r="B199">
+        <v>1.798853613228877e-05</v>
+      </c>
+    </row>
+    <row r="200">
+      <c r="A200">
+        <v>1.7052298983792977</v>
+      </c>
+      <c r="B200">
+        <v>2.6752557680311355e-20</v>
+      </c>
+    </row>
+    <row r="201">
+      <c r="A201">
+        <v>1.7149647956720488</v>
+      </c>
+      <c r="B201">
+        <v>2.6729596361220598e-20</v>
+      </c>
+    </row>
+    <row r="202">
+      <c r="A202">
+        <v>1.7252723339820208</v>
+      </c>
+      <c r="B202">
+        <v>2.6690131427214526e-20</v>
+      </c>
+    </row>
+    <row r="203">
+      <c r="A203">
+        <v>1.735007231274772</v>
+      </c>
+      <c r="B203">
+        <v>2.6640641323416483e-20</v>
+      </c>
+    </row>
+    <row r="204">
+      <c r="A204">
+        <v>1.7453147695847437</v>
+      </c>
+      <c r="B204">
+        <v>2.657718278272474e-20</v>
+      </c>
+    </row>
+    <row r="205">
+      <c r="A205">
+        <v>1.7550496668774951</v>
+      </c>
+      <c r="B205">
+        <v>2.6508299156363359e-20</v>
+      </c>
+    </row>
+    <row r="206">
+      <c r="A206">
+        <v>1.7653572051874669</v>
+      </c>
+      <c r="B206">
+        <v>2.6427296705241977e-20</v>
+      </c>
+    </row>
+    <row r="207">
+      <c r="A207">
+        <v>1.7750921024802182</v>
+      </c>
+      <c r="B207">
+        <v>2.6344336772311552e-20</v>
+      </c>
+    </row>
+    <row r="208">
+      <c r="A208">
+        <v>1.7848269997729693</v>
+      </c>
+      <c r="B208">
+        <v>2.6256117897682704e-20</v>
+      </c>
+    </row>
+    <row r="209">
+      <c r="A209">
+        <v>1.7951345380829411</v>
+      </c>
+      <c r="B209">
+        <v>2.6157977041333858e-20</v>
+      </c>
+    </row>
+    <row r="210">
+      <c r="A210">
+        <v>1.8048694353756922</v>
+      </c>
+      <c r="B210">
+        <v>2.606167715067699e-20</v>
+      </c>
+    </row>
+    <row r="211">
+      <c r="A211">
+        <v>1.8151769736856642</v>
+      </c>
+      <c r="B211">
+        <v>2.5956732153242127e-20</v>
+      </c>
+    </row>
+    <row r="212">
+      <c r="A212">
+        <v>1.8249118709784156</v>
+      </c>
+      <c r="B212">
+        <v>2.5855514477344823e-20</v>
+      </c>
+    </row>
+    <row r="213">
+      <c r="A213">
+        <v>1.8352194092883873</v>
+      </c>
+      <c r="B213">
+        <v>2.5746815660312595e-20</v>
+      </c>
+    </row>
+    <row r="214">
+      <c r="A214">
+        <v>1.8449543065811385</v>
+      </c>
+      <c r="B214">
+        <v>2.5643302671691386e-20</v>
+      </c>
+    </row>
+    <row r="215">
+      <c r="A215">
+        <v>1.8552618448911105</v>
+      </c>
+      <c r="B215">
+        <v>2.5533374749906883e-20</v>
+      </c>
+    </row>
+    <row r="216">
+      <c r="A216">
+        <v>1.8649967421838616</v>
+      </c>
+      <c r="B216">
+        <v>2.5429730739420038e-20</v>
+      </c>
+    </row>
+    <row r="217">
+      <c r="A217">
+        <v>1.8753042804938334</v>
+      </c>
+      <c r="B217">
+        <v>2.532065059658409e-20</v>
+      </c>
+    </row>
+  </sheetData>
+</worksheet>
 </file>
</xml_diff>